<commit_message>
check infinity interview categorization counts
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="27320" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-520" yWindow="4900" windowWidth="35080" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t>Table 1</t>
   </si>
@@ -118,16 +118,10 @@
     <t>AIC</t>
   </si>
   <si>
-    <t>Model comparisons done using Likelihood Ratio Tests. * p&lt;0.05, ** p&lt;0.01</t>
-  </si>
-  <si>
     <t>Table 3</t>
   </si>
   <si>
     <t>Regression models for predicting Endless knowledge on the Infinity Interview (N=122)</t>
-  </si>
-  <si>
-    <t>Age + Productivity (binary)</t>
   </si>
   <si>
     <t>Productivity
@@ -138,9 +132,6 @@
 (gradient)</t>
   </si>
   <si>
-    <t>Age + Productivity (gradient)</t>
-  </si>
-  <si>
     <t>**</t>
   </si>
   <si>
@@ -148,6 +139,60 @@
   </si>
   <si>
     <t>Model comparisons done using Likelihood Ratio Tests. None of the Initial Models explained significant variance beyond the Base Model.</t>
+  </si>
+  <si>
+    <t>Full Infinity knowledge</t>
+  </si>
+  <si>
+    <t>No infinity knowledge</t>
+  </si>
+  <si>
+    <t>Successor and Endless knowledge</t>
+  </si>
+  <si>
+    <t>Successor knowledge only</t>
+  </si>
+  <si>
+    <t>Endless knowledge only</t>
+  </si>
+  <si>
+    <t>Model comparisons done using Likelihood Ratio Tests against the base model. * p&lt;0.05, ** p&lt;0.01</t>
+  </si>
+  <si>
+    <t>Age + Productivity Group</t>
+  </si>
+  <si>
+    <t>Age + Productivity Gradient</t>
+  </si>
+  <si>
+    <t>Secondary Models</t>
+  </si>
+  <si>
+    <t>Age + IHC + HCNN</t>
+  </si>
+  <si>
+    <t>Age + IHC + Productivity Group</t>
+  </si>
+  <si>
+    <t>Age + IHC + Productivity Gradient</t>
+  </si>
+  <si>
+    <t>1.893**</t>
+  </si>
+  <si>
+    <t>0.535*</t>
+  </si>
+  <si>
+    <t>0.0179*</t>
+  </si>
+  <si>
+    <t>0.666**</t>
+  </si>
+  <si>
+    <t>1.329*</t>
+  </si>
+  <si>
+    <t>0.523*</t>
   </si>
 </sst>
 </file>
@@ -156,7 +201,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -274,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -334,6 +379,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -346,38 +427,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -666,15 +729,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I36" sqref="A30:I36"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="1.83203125" style="9" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
@@ -698,26 +761,26 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -747,21 +810,24 @@
         <v>40</v>
       </c>
       <c r="C5" s="14">
-        <v>0.50600000000000001</v>
+        <f>B5/79</f>
+        <v>0.50632911392405067</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="10">
         <v>12</v>
       </c>
       <c r="F5" s="14">
-        <v>0.27900000000000003</v>
+        <f>E5/43</f>
+        <v>0.27906976744186046</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="10">
         <v>52</v>
       </c>
       <c r="I5" s="14">
-        <v>0.42599999999999999</v>
+        <f>H5/122</f>
+        <v>0.42622950819672129</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -772,21 +838,24 @@
         <v>30</v>
       </c>
       <c r="C6" s="16">
-        <v>0.38</v>
+        <f>B6/79</f>
+        <v>0.379746835443038</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="7">
         <v>4</v>
       </c>
       <c r="F6" s="16">
-        <v>9.2999999999999999E-2</v>
+        <f>E6/43</f>
+        <v>9.3023255813953487E-2</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="7">
         <v>34</v>
       </c>
       <c r="I6" s="16">
-        <v>0.27900000000000003</v>
+        <f>H6/122</f>
+        <v>0.27868852459016391</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -811,192 +880,402 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="38"/>
+    </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="8">
+        <v>29</v>
+      </c>
+      <c r="C13" s="17">
+        <f>B13/79</f>
+        <v>0.36708860759493672</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
+        <v>30</v>
+      </c>
+      <c r="F13" s="17">
+        <f>E13/43</f>
+        <v>0.69767441860465118</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8">
+        <v>59</v>
+      </c>
+      <c r="I13" s="17">
+        <f>H13/122</f>
+        <v>0.48360655737704916</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="10">
+        <v>20</v>
+      </c>
+      <c r="C14" s="17">
+        <f t="shared" ref="C14:C16" si="0">B14/79</f>
+        <v>0.25316455696202533</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="10">
+        <v>9</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" ref="F14:F16" si="1">E14/43</f>
+        <v>0.20930232558139536</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="10">
+        <v>29</v>
+      </c>
+      <c r="I14" s="14">
+        <f>H14/122</f>
+        <v>0.23770491803278687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8">
+        <v>10</v>
+      </c>
+      <c r="C15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.12658227848101267</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="F15" s="17">
+        <f t="shared" si="1"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="8">
+        <v>11</v>
+      </c>
+      <c r="I15" s="17">
+        <f>H15/122</f>
+        <v>9.0163934426229511E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="7">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16">
+        <f t="shared" si="0"/>
+        <v>0.25316455696202533</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="16">
+        <f t="shared" si="1"/>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="7">
+        <v>23</v>
+      </c>
+      <c r="I16" s="16">
+        <f>H16/122</f>
+        <v>0.18852459016393441</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="25" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="25" t="s">
+      <c r="F22" s="38"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="7" t="s">
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="36"/>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="H24" s="13"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B25" s="10">
         <v>40</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C25" s="14">
         <v>0.50600000000000001</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="10">
+      <c r="D25" s="14"/>
+      <c r="E25" s="10">
         <v>12</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F25" s="14">
         <v>0.27900000000000003</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="10">
+      <c r="G25" s="14"/>
+      <c r="H25" s="10">
         <v>52</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I25" s="14">
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B26" s="10">
         <v>39</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C26" s="14">
         <v>0.49099999999999999</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="10">
+      <c r="D26" s="14"/>
+      <c r="E26" s="10">
         <v>31</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F26" s="14">
         <v>0.72099999999999997</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="10">
+      <c r="G26" s="14"/>
+      <c r="H26" s="10">
         <v>70</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I26" s="14">
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B28" s="10">
         <v>30</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C28" s="14">
         <v>0.38</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="10">
+      <c r="D28" s="14"/>
+      <c r="E28" s="10">
         <v>4</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F28" s="14">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="10">
+      <c r="G28" s="14"/>
+      <c r="H28" s="10">
         <v>34</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I28" s="14">
         <v>0.27900000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B29" s="8">
         <v>49</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C29" s="17">
         <v>0.62</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="7">
+      <c r="D29" s="17"/>
+      <c r="E29" s="8">
         <v>39</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F29" s="17">
         <v>0.80700000000000005</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="7">
+      <c r="G29" s="17"/>
+      <c r="H29" s="8">
         <v>88</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I29" s="17">
         <v>0.72099999999999997</v>
       </c>
     </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="23"/>
+      <c r="B31" s="7">
+        <v>16</v>
+      </c>
+      <c r="C31" s="16">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="7">
+        <v>3</v>
+      </c>
+      <c r="F31" s="16">
+        <v>6.9760000000000003E-2</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="7">
+        <v>19</v>
+      </c>
+      <c r="I31" s="16">
+        <v>0.15570000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1013,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,25 +1322,25 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1072,10 +1351,10 @@
         <v>24</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
@@ -1094,18 +1373,18 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="24">
         <v>0.34200000000000003</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="34">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="31">
         <v>-81.539000000000001</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="31">
         <v>167.077</v>
       </c>
     </row>
@@ -1113,33 +1392,33 @@
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="26">
         <v>0.313</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="35">
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="32">
         <v>-81.503</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="32">
         <v>169.006</v>
       </c>
     </row>
@@ -1147,72 +1426,80 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="24">
         <v>0.245</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24">
         <v>0.27100000000000002</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="34">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="31">
         <v>-80.61</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="31">
         <v>167.221</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="32">
+        <v>41</v>
+      </c>
+      <c r="B10" s="29">
         <v>0.14899999999999999</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29">
         <v>0.81599999999999995</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="36">
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="33">
         <v>-79.977000000000004</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="33">
         <v>165.95400000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0.217</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="30">
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="34">
+        <v>-81.072000000000003</v>
+      </c>
+      <c r="I11" s="34">
+        <v>168.143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="33">
-        <v>0.20979999999999999</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="37">
-        <v>-81.016000000000005</v>
-      </c>
-      <c r="I11" s="37">
-        <v>168.03299999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
+      <c r="A16" s="27"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1233,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,12 +1536,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1266,24 +1553,24 @@
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1294,10 +1581,10 @@
         <v>24</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
@@ -1316,18 +1603,18 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="24">
         <v>0.70699999999999996</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="34">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="31">
         <v>-66.655000000000001</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="31">
         <v>137.31100000000001</v>
       </c>
     </row>
@@ -1335,35 +1622,35 @@
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="26">
         <v>0.40699999999999997</v>
       </c>
-      <c r="C8" s="29">
-        <v>0.66600000000000004</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="35">
+      <c r="C8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="32">
         <v>-62.81</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="32">
         <v>131.619</v>
       </c>
     </row>
@@ -1371,140 +1658,165 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="27">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27">
-        <v>0.504</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="34">
+      <c r="B9" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="31">
         <v>-63.884</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="31">
         <v>133.767</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="32">
+      <c r="A10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="29">
         <v>0.44600000000000001</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32">
-        <v>1.329</v>
-      </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="36">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="33">
         <v>-64.094999999999999</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="33">
         <v>134.19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="28">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
-        <v>1.962</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="37">
+      <c r="A11" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="29">
+        <v>0.313</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="33">
         <v>-62.311999999999998</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="33">
         <v>130.624</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="29">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.17299999999999999</v>
+      </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="H13" s="33">
+        <v>-62.642000000000003</v>
+      </c>
+      <c r="I13" s="33">
+        <v>133.28399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="29">
+        <v>0.315</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="33">
+        <v>-62.058999999999997</v>
+      </c>
+      <c r="I14" s="33">
+        <v>132.11799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="42">
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="42">
+        <v>1.3282</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33">
+        <v>130.59</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
-        <v>28</v>
+      <c r="A16" s="4"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated figures and regression tables
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-520" yWindow="4900" windowWidth="35080" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="3" r:id="rId2"/>
     <sheet name="Table3" sheetId="5" r:id="rId3"/>
+    <sheet name="Table4" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
   <si>
     <t>Table 1</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Age + HCNN</t>
   </si>
   <si>
-    <t>Predictor Estimates (ß)</t>
-  </si>
-  <si>
     <t>IHC</t>
   </si>
   <si>
@@ -110,9 +108,6 @@
   </si>
   <si>
     <t>Summary statistics</t>
-  </si>
-  <si>
-    <t>Loglikelihood</t>
   </si>
   <si>
     <t>AIC</t>
@@ -132,15 +127,6 @@
 (gradient)</t>
   </si>
   <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>Model comparisons done using Likelihood Ratio Tests. None of the Initial Models explained significant variance beyond the Base Model.</t>
-  </si>
-  <si>
     <t>Full Infinity knowledge</t>
   </si>
   <si>
@@ -156,9 +142,6 @@
     <t>Endless knowledge only</t>
   </si>
   <si>
-    <t>Model comparisons done using Likelihood Ratio Tests against the base model. * p&lt;0.05, ** p&lt;0.01</t>
-  </si>
-  <si>
     <t>Age + Productivity Group</t>
   </si>
   <si>
@@ -177,9 +160,6 @@
     <t>Age + IHC + Productivity Gradient</t>
   </si>
   <si>
-    <t>1.893**</t>
-  </si>
-  <si>
     <t>0.535*</t>
   </si>
   <si>
@@ -193,6 +173,282 @@
   </si>
   <si>
     <t>0.523*</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Regression models for predicting Full Infinity knowledge on the Infinity Interview (N=122)</t>
+  </si>
+  <si>
+    <t>0.567*</t>
+  </si>
+  <si>
+    <t>0.752**</t>
+  </si>
+  <si>
+    <t>0.609*</t>
+  </si>
+  <si>
+    <t>0.572*</t>
+  </si>
+  <si>
+    <t>0.488*</t>
+  </si>
+  <si>
+    <t>0.707**</t>
+  </si>
+  <si>
+    <t>1.962**</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Nagelkerke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Loglikelihood </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <t>-62.81**</t>
+  </si>
+  <si>
+    <t>-63.88*</t>
+  </si>
+  <si>
+    <t>-64.10*</t>
+  </si>
+  <si>
+    <t>-62.31**</t>
+  </si>
+  <si>
+    <t>Coefficient Estimates (ß)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Coefficients were tested using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">-tests. Model comparisons done using Likelihood Ratio Tests. * </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;0.05, ** </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Each initial model was compared against the base model. None of the Initial Models explained significant variance beyond the Base Model.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Coefficients were tested using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-tests. Model</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">comparisons done using Likelihood Ratio Tests. * p&lt;0.05, ** p&lt;0.01
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Each initial model was compared against the base model. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Each Secondary model was compared against the "Age + IHC" initial model. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -203,7 +459,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,6 +512,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -319,7 +597,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -415,6 +693,24 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -427,20 +723,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -731,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A3" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
@@ -761,26 +1059,26 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="38"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -897,26 +1195,26 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="38"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
@@ -940,7 +1238,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="8">
         <v>29</v>
@@ -968,7 +1266,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" s="10">
         <v>20</v>
@@ -996,7 +1294,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" s="8">
         <v>10</v>
@@ -1023,8 +1321,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
-        <v>37</v>
+      <c r="A16" s="37" t="s">
+        <v>32</v>
       </c>
       <c r="B16" s="7">
         <v>20</v>
@@ -1067,26 +1365,26 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="38"/>
+      <c r="F22" s="44"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="38"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
@@ -1227,8 +1525,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
-        <v>35</v>
+      <c r="A30" s="36" t="s">
+        <v>30</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="17"/>
@@ -1290,26 +1588,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
@@ -1319,57 +1619,61 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="B3" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="38"/>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="H3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1387,8 +1691,11 @@
       <c r="I6" s="31">
         <v>167.077</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="51">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -1400,8 +1707,9 @@
       <c r="G7" s="24"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1421,8 +1729,11 @@
       <c r="I8" s="32">
         <v>169.006</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="51">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1442,10 +1753,13 @@
       <c r="I9" s="31">
         <v>167.221</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="51">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="29">
         <v>0.14899999999999999</v>
@@ -1463,10 +1777,13 @@
       <c r="I10" s="33">
         <v>165.95400000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="30">
         <v>0.217</v>
@@ -1484,13 +1801,25 @@
       <c r="I11" s="34">
         <v>168.143</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="51">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1502,10 +1831,11 @@
       <c r="I16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="A12:J12"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1520,28 +1850,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1549,62 +1881,66 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="B3" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="38"/>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="H3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="24">
-        <v>0.70699999999999996</v>
+      <c r="B6" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1612,13 +1948,16 @@
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="31">
-        <v>-66.655000000000001</v>
+        <v>-66.66</v>
       </c>
       <c r="I6" s="31">
         <v>137.31100000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="39">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -1630,8 +1969,9 @@
       <c r="G7" s="24"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="39"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1639,47 +1979,49 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
-      <c r="G8" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="32">
-        <v>-62.81</v>
+      <c r="G8" s="26"/>
+      <c r="H8" s="45" t="s">
+        <v>57</v>
       </c>
       <c r="I8" s="32">
         <v>131.619</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="39">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="31">
-        <v>-63.884</v>
+      <c r="G9" s="24"/>
+      <c r="H9" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="I9" s="31">
         <v>133.767</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="39">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="29">
         <v>0.44600000000000001</v>
@@ -1687,45 +2029,47 @@
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F10" s="29"/>
-      <c r="G10" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="33">
-        <v>-64.094999999999999</v>
+      <c r="G10" s="29"/>
+      <c r="H10" s="47" t="s">
+        <v>59</v>
       </c>
       <c r="I10" s="33">
         <v>134.19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="39">
+        <v>0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="29">
-        <v>0.313</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="33">
-        <v>-62.311999999999998</v>
+        <v>54</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="I11" s="33">
         <v>130.624</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="39">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -1735,10 +2079,11 @@
       <c r="G12" s="29"/>
       <c r="H12" s="33"/>
       <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="50"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B13" s="29">
         <v>0.41099999999999998</v>
@@ -1758,16 +2103,19 @@
       <c r="I13" s="33">
         <v>133.28399999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
-        <v>45</v>
+      <c r="J13" s="39">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="38" t="s">
+        <v>39</v>
       </c>
       <c r="B14" s="29">
         <v>0.315</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29">
@@ -1781,49 +2129,321 @@
       <c r="I14" s="33">
         <v>132.11799999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="C15" s="42">
-        <v>0.42070000000000002</v>
+      <c r="J14" s="39">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="39">
+        <v>0.249</v>
+      </c>
+      <c r="C15" s="39">
+        <v>0.40500000000000003</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="42">
-        <v>1.3282</v>
+      <c r="F15" s="39">
+        <v>1.3877999999999999</v>
       </c>
       <c r="G15" s="29"/>
-      <c r="H15" s="33"/>
+      <c r="H15" s="33">
+        <v>-61.134999999999998</v>
+      </c>
       <c r="I15" s="33">
-        <v>130.59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
-        <v>40</v>
-      </c>
+        <v>130.47</v>
+      </c>
+      <c r="J15" s="39">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="49" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="31">
+        <v>-54.354999999999997</v>
+      </c>
+      <c r="I6" s="31">
+        <v>112.711</v>
+      </c>
+      <c r="J6" s="51">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="32">
+        <v>-53.375</v>
+      </c>
+      <c r="I8" s="32">
+        <v>112.75</v>
+      </c>
+      <c r="J8" s="51">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="31">
+        <v>-53.04</v>
+      </c>
+      <c r="I9" s="31">
+        <v>112.08</v>
+      </c>
+      <c r="J9" s="51">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="33">
+        <v>-53.497</v>
+      </c>
+      <c r="I10" s="33">
+        <v>112.995</v>
+      </c>
+      <c r="J10" s="51">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="30">
+        <v>1.2729999999999999</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="34">
+        <v>-52.970999999999997</v>
+      </c>
+      <c r="I11" s="34">
+        <v>111.94199999999999</v>
+      </c>
+      <c r="J11" s="51">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
coded reminder prompts and recoveries
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyichu/Sites/recursion/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA62C3-75B0-7741-876E-5BB24C3E105C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table2" sheetId="3" r:id="rId2"/>
-    <sheet name="Table3" sheetId="5" r:id="rId3"/>
-    <sheet name="Table4" sheetId="7" r:id="rId4"/>
+    <sheet name="Table3" sheetId="3" r:id="rId2"/>
+    <sheet name="Table4" sheetId="5" r:id="rId3"/>
+    <sheet name="Table5" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>Table 1</t>
   </si>
@@ -163,9 +169,6 @@
     <t>0.535*</t>
   </si>
   <si>
-    <t>0.0179*</t>
-  </si>
-  <si>
     <t>0.666**</t>
   </si>
   <si>
@@ -197,9 +200,6 @@
   </si>
   <si>
     <t>0.707**</t>
-  </si>
-  <si>
-    <t>1.962**</t>
   </si>
   <si>
     <r>
@@ -251,10 +251,25 @@
     <t>-64.10*</t>
   </si>
   <si>
-    <t>-62.31**</t>
-  </si>
-  <si>
     <t>Coefficient Estimates (ß)</t>
+  </si>
+  <si>
+    <t>0.504*</t>
+  </si>
+  <si>
+    <t>1.893**</t>
+  </si>
+  <si>
+    <t>-62.49**</t>
+  </si>
+  <si>
+    <t>Infinity knowledge classifications</t>
+  </si>
+  <si>
+    <t>% (of 122)</t>
+  </si>
+  <si>
+    <t>Frequency of infinity knowledge</t>
   </si>
   <si>
     <r>
@@ -267,64 +282,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Coefficients were tested using </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">-tests. Model comparisons done using Likelihood Ratio Tests. * </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;0.05, ** </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;0.01</t>
+      <t>HCNN: Highest Contiguous Next Number.</t>
     </r>
     <r>
       <rPr>
@@ -339,6 +297,83 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Coefficients were tested using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">-tests. Model comparisons done using Likelihood Ratio Tests. * </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;0.05, ** </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
@@ -369,6 +404,26 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>HCNN: Highest Contiguous Next Number.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t xml:space="preserve">Coefficients were tested using </t>
     </r>
     <r>
@@ -450,16 +505,19 @@
       <t xml:space="preserve">Each Secondary model was compared against the "Age + IHC" initial model. </t>
     </r>
   </si>
+  <si>
+    <t>Table 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,6 +595,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -584,7 +649,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -596,8 +661,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -711,18 +777,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,17 +785,62 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -753,12 +852,16 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1026,19 +1129,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A3" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="1.83203125" style="9" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1059,26 +1164,26 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="44"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="44"/>
+      <c r="I3" s="61"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1195,26 +1300,26 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="44"/>
+      <c r="I11" s="61"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1348,228 +1453,437 @@
         <v>0.18852459016393441</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="61"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="61"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="20"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="43" t="s">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10">
+        <v>40</v>
+      </c>
+      <c r="C23" s="56">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="10">
         <v>12</v>
       </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="44"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>6</v>
+      <c r="F23" s="56">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="10">
+        <v>52</v>
+      </c>
+      <c r="I23" s="56">
+        <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="9"/>
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="10">
+        <v>39</v>
+      </c>
+      <c r="C24" s="56">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="10">
+        <v>31</v>
+      </c>
+      <c r="F24" s="56">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="10">
+        <v>70</v>
+      </c>
+      <c r="I24" s="56">
+        <v>0.57399999999999995</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="10">
-        <v>40</v>
-      </c>
-      <c r="C25" s="14">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="10">
-        <v>12</v>
-      </c>
-      <c r="F25" s="14">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="10">
-        <v>52</v>
-      </c>
-      <c r="I25" s="14">
-        <v>0.42599999999999999</v>
-      </c>
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="15"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="57"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="10">
-        <v>39</v>
-      </c>
-      <c r="C26" s="14">
-        <v>0.49099999999999999</v>
+        <v>30</v>
+      </c>
+      <c r="C26" s="56">
+        <v>0.38</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="10">
-        <v>31</v>
-      </c>
-      <c r="F26" s="14">
-        <v>0.72099999999999997</v>
+        <v>4</v>
+      </c>
+      <c r="F26" s="56">
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="10">
-        <v>70</v>
-      </c>
-      <c r="I26" s="14">
-        <v>0.57399999999999995</v>
+        <v>34</v>
+      </c>
+      <c r="I26" s="56">
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="15"/>
+      <c r="A27" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="8">
+        <v>49</v>
+      </c>
+      <c r="C27" s="54">
+        <v>0.62</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="8">
+        <v>39</v>
+      </c>
+      <c r="F27" s="54">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="8">
+        <v>88</v>
+      </c>
+      <c r="I27" s="54">
+        <v>0.72099999999999997</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="10">
+      <c r="A28" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="14">
-        <v>0.38</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="10">
-        <v>4</v>
-      </c>
-      <c r="F28" s="14">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="10">
-        <v>34</v>
-      </c>
-      <c r="I28" s="14">
-        <v>0.27900000000000003</v>
-      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="8">
-        <v>49</v>
-      </c>
-      <c r="C29" s="17">
-        <v>0.62</v>
+        <v>20</v>
+      </c>
+      <c r="C29" s="54">
+        <f>B29/79</f>
+        <v>0.25316455696202533</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="8">
-        <v>39</v>
-      </c>
-      <c r="F29" s="17">
-        <v>0.80700000000000005</v>
+        <v>3</v>
+      </c>
+      <c r="F29" s="54">
+        <f>E29/43</f>
+        <v>6.9767441860465115E-2</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="8">
+        <v>23</v>
+      </c>
+      <c r="I29" s="54">
+        <f>H29/122</f>
+        <v>0.18852459016393441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7">
+        <v>59</v>
+      </c>
+      <c r="C30" s="55">
+        <f>B30/79</f>
+        <v>0.74683544303797467</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="7">
+        <v>40</v>
+      </c>
+      <c r="F30" s="55">
+        <f>E30/43</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="7">
+        <v>99</v>
+      </c>
+      <c r="I30" s="55">
+        <f>H30/122</f>
+        <v>0.81147540983606559</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="61"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="61"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="59"/>
+      <c r="B37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="10">
+        <v>52</v>
+      </c>
+      <c r="C38" s="49">
+        <f>B38/122</f>
+        <v>0.42622950819672129</v>
+      </c>
+      <c r="E38" s="10">
+        <v>70</v>
+      </c>
+      <c r="F38" s="51">
+        <f>E38/122</f>
+        <v>0.57377049180327866</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="7">
+        <v>34</v>
+      </c>
+      <c r="C39" s="50">
+        <f>B39/122</f>
+        <v>0.27868852459016391</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="7">
         <v>88</v>
       </c>
-      <c r="I29" s="17">
-        <v>0.72099999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="7">
-        <v>16</v>
-      </c>
-      <c r="C31" s="16">
-        <v>0.20250000000000001</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="7">
-        <v>3</v>
-      </c>
-      <c r="F31" s="16">
-        <v>6.9760000000000003E-2</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="7">
-        <v>19</v>
-      </c>
-      <c r="I31" s="16">
-        <v>0.15570000000000001</v>
-      </c>
+      <c r="F39" s="50">
+        <f>E39/122</f>
+        <v>0.72131147540983609</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="28"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="47"/>
+      <c r="B44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="8">
+        <v>59</v>
+      </c>
+      <c r="C45" s="54">
+        <f>B45/122</f>
+        <v>0.48360655737704916</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="10">
+        <v>29</v>
+      </c>
+      <c r="C46" s="54">
+        <f t="shared" ref="C46:C48" si="2">B46/122</f>
+        <v>0.23770491803278687</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="8">
+        <v>11</v>
+      </c>
+      <c r="C47" s="54">
+        <f t="shared" si="2"/>
+        <v>9.0163934426229511E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="7">
+        <v>23</v>
+      </c>
+      <c r="C48" s="55">
+        <f t="shared" si="2"/>
+        <v>0.18852459016393441</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
@@ -1587,11 +1901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,7 +1920,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1623,25 +1937,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="B3" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1659,13 +1973,13 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1691,7 +2005,7 @@
       <c r="I6" s="31">
         <v>167.077</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="46">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
@@ -1707,7 +2021,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="51"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1729,7 +2043,7 @@
       <c r="I8" s="32">
         <v>169.006</v>
       </c>
-      <c r="J8" s="51">
+      <c r="J8" s="46">
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
@@ -1753,7 +2067,7 @@
       <c r="I9" s="31">
         <v>167.221</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="46">
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
@@ -1777,7 +2091,7 @@
       <c r="I10" s="33">
         <v>165.95400000000001</v>
       </c>
-      <c r="J10" s="51">
+      <c r="J10" s="46">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -1801,23 +2115,23 @@
       <c r="I11" s="34">
         <v>168.143</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="46">
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
@@ -1849,11 +2163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A16" sqref="A16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1868,7 +2182,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1885,25 +2199,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="B3" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1921,13 +2235,13 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1940,7 +2254,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1979,14 +2293,14 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="45" t="s">
-        <v>57</v>
+      <c r="H8" s="41" t="s">
+        <v>55</v>
       </c>
       <c r="I8" s="32">
         <v>131.619</v>
@@ -2004,13 +2318,13 @@
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="46" t="s">
-        <v>58</v>
+      <c r="H9" s="42" t="s">
+        <v>56</v>
       </c>
       <c r="I9" s="31">
         <v>133.767</v>
@@ -2029,12 +2343,12 @@
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="47" t="s">
-        <v>59</v>
+      <c r="H10" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="I10" s="33">
         <v>134.19</v>
@@ -2054,11 +2368,11 @@
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G11" s="29"/>
-      <c r="H11" s="47" t="s">
-        <v>60</v>
+      <c r="H11" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="I11" s="33">
         <v>130.624</v>
@@ -2079,7 +2393,7 @@
       <c r="G12" s="29"/>
       <c r="H12" s="33"/>
       <c r="I12" s="33"/>
-      <c r="J12" s="50"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -2115,7 +2429,7 @@
         <v>0.315</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29">
@@ -2159,19 +2473,19 @@
         <v>0.23699999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="49" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+    <row r="16" spans="1:10" s="44" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2192,11 +2506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2211,12 +2525,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2228,25 +2542,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="B3" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2264,13 +2578,13 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2283,7 +2597,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2296,7 +2610,7 @@
       <c r="I6" s="31">
         <v>112.711</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="46">
         <v>0.12</v>
       </c>
     </row>
@@ -2312,14 +2626,14 @@
       <c r="G7" s="24"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="51"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="26">
         <v>0.38500000000000001</v>
@@ -2334,7 +2648,7 @@
       <c r="I8" s="32">
         <v>112.75</v>
       </c>
-      <c r="J8" s="51">
+      <c r="J8" s="46">
         <v>0.14299999999999999</v>
       </c>
     </row>
@@ -2343,7 +2657,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24">
@@ -2358,7 +2672,7 @@
       <c r="I9" s="31">
         <v>112.08</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="46">
         <v>0.151</v>
       </c>
     </row>
@@ -2367,7 +2681,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -2382,7 +2696,7 @@
       <c r="I10" s="33">
         <v>112.995</v>
       </c>
-      <c r="J10" s="51">
+      <c r="J10" s="46">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -2391,7 +2705,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -2406,23 +2720,23 @@
       <c r="I11" s="34">
         <v>111.94199999999999</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="46">
         <v>0.153</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>

</xml_diff>

<commit_message>
reknitted for today's update
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyichu/Sites/recursion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA62C3-75B0-7741-876E-5BB24C3E105C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F13709-94A1-284F-A700-CECD6307EA5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table3" sheetId="3" r:id="rId2"/>
-    <sheet name="Table4" sheetId="5" r:id="rId3"/>
-    <sheet name="Table5" sheetId="7" r:id="rId4"/>
+    <sheet name="Table2" sheetId="3" r:id="rId2"/>
+    <sheet name="Table3" sheetId="5" r:id="rId3"/>
+    <sheet name="Table4" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>Table 1</t>
   </si>
@@ -83,9 +83,6 @@
 (N=122)</t>
   </si>
   <si>
-    <t>Table 2</t>
-  </si>
-  <si>
     <t>Regression models for predicting Successor knowledge on the Infinity Interview (N=122)</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>0.523*</t>
-  </si>
-  <si>
-    <t>Table 4</t>
   </si>
   <si>
     <t>Regression models for predicting Full Infinity knowledge on the Infinity Interview (N=122)</t>
@@ -507,6 +501,18 @@
   </si>
   <si>
     <t>Table 5</t>
+  </si>
+  <si>
+    <t>Has Successor knowledge</t>
+  </si>
+  <si>
+    <t>Has Endless knowledge</t>
+  </si>
+  <si>
+    <t>No Infinity knowledge</t>
+  </si>
+  <si>
+    <t>Table 2</t>
   </si>
 </sst>
 </file>
@@ -663,7 +669,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -823,6 +829,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1130,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A45" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,26 +1173,26 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="61"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="61"/>
+      <c r="I3" s="62"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1300,26 +1309,26 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="61"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="60" t="s">
+      <c r="H11" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="61"/>
+      <c r="I11" s="62"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1343,7 +1352,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="8">
         <v>29</v>
@@ -1371,7 +1380,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="10">
         <v>20</v>
@@ -1399,7 +1408,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="8">
         <v>10</v>
@@ -1427,7 +1436,7 @@
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="7">
         <v>20</v>
@@ -1455,7 +1464,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1470,26 +1479,26 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="62"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="61"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="60" t="s">
+      <c r="H20" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="61"/>
+      <c r="I20" s="62"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="59"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
@@ -1515,8 +1524,14 @@
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -1631,7 +1646,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="54"/>
@@ -1705,7 +1720,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -1714,33 +1729,33 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="61"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="61"/>
+      <c r="F36" s="62"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="59"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1805,7 +1820,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1821,7 +1836,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="8">
         <v>59</v>
@@ -1833,7 +1848,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="10">
         <v>29</v>
@@ -1845,7 +1860,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="8">
         <v>11</v>
@@ -1857,7 +1872,7 @@
     </row>
     <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="7">
         <v>23</v>
@@ -1867,15 +1882,175 @@
         <v>0.18852459016393441</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="52"/>
       <c r="B49" s="53"/>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="62"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="62"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="62"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="60"/>
+      <c r="B54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="8">
+        <v>29</v>
+      </c>
+      <c r="C55" s="54">
+        <f>B55/79</f>
+        <v>0.36708860759493672</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8">
+        <v>30</v>
+      </c>
+      <c r="F55" s="54">
+        <f>E55/43</f>
+        <v>0.69767441860465118</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8">
+        <v>59</v>
+      </c>
+      <c r="I55" s="54">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="10">
+        <v>40</v>
+      </c>
+      <c r="C56" s="56">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="10">
+        <v>12</v>
+      </c>
+      <c r="F56" s="56">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G56" s="14"/>
+      <c r="H56" s="10">
+        <v>52</v>
+      </c>
+      <c r="I56" s="56">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" s="10">
+        <v>30</v>
+      </c>
+      <c r="C57" s="56">
+        <v>0.38</v>
+      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="10">
+        <v>4</v>
+      </c>
+      <c r="F57" s="56">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="H57" s="10">
+        <v>34</v>
+      </c>
+      <c r="I57" s="56">
+        <v>0.27900000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="7">
+        <v>20</v>
+      </c>
+      <c r="C58" s="55">
+        <f>B58/79</f>
+        <v>0.25316455696202533</v>
+      </c>
+      <c r="D58" s="16"/>
+      <c r="E58" s="7">
+        <v>3</v>
+      </c>
+      <c r="F58" s="55">
+        <f>E58/43</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="G58" s="16"/>
+      <c r="H58" s="7">
+        <v>23</v>
+      </c>
+      <c r="I58" s="55">
+        <f>H58/122</f>
+        <v>0.18852459016393441</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
+  <mergeCells count="19">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
@@ -1888,6 +2063,13 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1904,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:J12"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A11" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1920,12 +2102,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1937,59 +2119,59 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
+      <c r="A3" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="H3" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="24">
         <v>0.34200000000000003</v>
@@ -2011,7 +2193,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -2025,7 +2207,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="26">
         <v>0.313</v>
@@ -2049,7 +2231,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="24">
         <v>0.245</v>
@@ -2073,7 +2255,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="29">
         <v>0.14899999999999999</v>
@@ -2097,7 +2279,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="30">
         <v>0.217</v>
@@ -2120,18 +2302,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
+      <c r="A12" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
@@ -2166,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J16"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2182,12 +2364,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2199,62 +2381,62 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
+      <c r="A3" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="H3" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2273,7 +2455,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -2287,20 +2469,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="26">
         <v>0.40699999999999997</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="32">
         <v>131.619</v>
@@ -2311,20 +2493,20 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I9" s="31">
         <v>133.767</v>
@@ -2335,7 +2517,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="29">
         <v>0.44600000000000001</v>
@@ -2343,12 +2525,12 @@
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" s="33">
         <v>134.19</v>
@@ -2359,7 +2541,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="29">
         <v>0.30499999999999999</v>
@@ -2368,11 +2550,11 @@
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" s="33">
         <v>130.624</v>
@@ -2383,7 +2565,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2397,7 +2579,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="29">
         <v>0.41099999999999998</v>
@@ -2423,13 +2605,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="29">
         <v>0.315</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29">
@@ -2449,7 +2631,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="39">
         <v>0.249</v>
@@ -2474,18 +2656,18 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="44" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
+      <c r="A16" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2510,7 +2692,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2525,12 +2707,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2542,62 +2724,62 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
+      <c r="A3" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="H3" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2616,7 +2798,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -2630,10 +2812,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="26">
         <v>0.38500000000000001</v>
@@ -2654,10 +2836,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24">
@@ -2678,10 +2860,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -2702,10 +2884,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -2725,18 +2907,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
+      <c r="A12" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>

</xml_diff>

<commit_message>
use colorblind palette and update regression tables excel file; corrected typos in regression tables
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyichu/Sites/recursion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F13709-94A1-284F-A700-CECD6307EA5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FD1C20-FF0A-1441-B3DF-B3869E1A668F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33140" yWindow="-2260" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
   <si>
     <t>Table 1</t>
   </si>
@@ -101,13 +101,7 @@
     <t>Age + IHC</t>
   </si>
   <si>
-    <t>Age + HCNN</t>
-  </si>
-  <si>
     <t>IHC</t>
-  </si>
-  <si>
-    <t>HCNN</t>
   </si>
   <si>
     <t>Summary statistics</t>
@@ -154,27 +148,15 @@
     <t>Secondary Models</t>
   </si>
   <si>
-    <t>Age + IHC + HCNN</t>
-  </si>
-  <si>
     <t>Age + IHC + Productivity Group</t>
   </si>
   <si>
     <t>Age + IHC + Productivity Gradient</t>
   </si>
   <si>
-    <t>0.535*</t>
-  </si>
-  <si>
     <t>0.666**</t>
   </si>
   <si>
-    <t>1.329*</t>
-  </si>
-  <si>
-    <t>0.523*</t>
-  </si>
-  <si>
     <t>Regression models for predicting Full Infinity knowledge on the Infinity Interview (N=122)</t>
   </si>
   <si>
@@ -184,15 +166,6 @@
     <t>0.752**</t>
   </si>
   <si>
-    <t>0.609*</t>
-  </si>
-  <si>
-    <t>0.572*</t>
-  </si>
-  <si>
-    <t>0.488*</t>
-  </si>
-  <si>
     <t>0.707**</t>
   </si>
   <si>
@@ -239,21 +212,9 @@
     <t>-62.81**</t>
   </si>
   <si>
-    <t>-63.88*</t>
-  </si>
-  <si>
-    <t>-64.10*</t>
-  </si>
-  <si>
     <t>Coefficient Estimates (ß)</t>
   </si>
   <si>
-    <t>0.504*</t>
-  </si>
-  <si>
-    <t>1.893**</t>
-  </si>
-  <si>
     <t>-62.49**</t>
   </si>
   <si>
@@ -266,6 +227,46 @@
     <t>Frequency of infinity knowledge</t>
   </si>
   <si>
+    <t>Has Successor knowledge</t>
+  </si>
+  <si>
+    <t>Has Endless knowledge</t>
+  </si>
+  <si>
+    <t>No Infinity knowledge</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Next Number
+accuracy</t>
+  </si>
+  <si>
+    <t>Age + Next Number accuracy</t>
+  </si>
+  <si>
+    <t>Age + IHC + Next Number accuracy</t>
+  </si>
+  <si>
+    <t>0.849**</t>
+  </si>
+  <si>
+    <t>0.693**</t>
+  </si>
+  <si>
+    <t>1.636**</t>
+  </si>
+  <si>
+    <t>-62.89**</t>
+  </si>
+  <si>
+    <t>-62.69**</t>
+  </si>
+  <si>
+    <t>-53.04*</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Notes. </t>
     </r>
@@ -276,7 +277,64 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>HCNN: Highest Contiguous Next Number.</t>
+      <t xml:space="preserve">Coefficients were tested using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">-tests. Model comparisons done using Likelihood Ratio Tests. * </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">p &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">0.05, ** </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt; 0.01</t>
     </r>
     <r>
       <rPr>
@@ -291,16 +349,41 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Coefficients were tested using </t>
-    </r>
-    <r>
-      <rPr>
         <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Each initial model was compared against the base model.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Coefficients were compared against 0 using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
@@ -315,45 +398,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">-tests. Model comparisons done using Likelihood Ratio Tests. * </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;0.05, ** </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;0.01</t>
+      <t>-tests. Model comparisons done using Likelihood Ratio Tests. * p &lt; 0.05, ** p &lt; 0.01</t>
     </r>
     <r>
       <rPr>
@@ -388,6 +433,9 @@
     </r>
   </si>
   <si>
+    <t>Table 4</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Notes. </t>
     </r>
@@ -398,7 +446,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>HCNN: Highest Contiguous Next Number.</t>
+      <t xml:space="preserve">Coefficients were compared against 0 using </t>
     </r>
     <r>
       <rPr>
@@ -408,17 +456,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Coefficients were tested using </t>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-tests. Model</t>
     </r>
     <r>
       <rPr>
@@ -428,16 +475,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-tests. Model</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">comparisons done using Likelihood Ratio Tests. * </t>
     </r>
     <r>
       <rPr>
@@ -447,16 +494,35 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">comparisons done using Likelihood Ratio Tests. * p&lt;0.05, ** p&lt;0.01
+      <t xml:space="preserve">p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt; 0.05, ** </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt; 0.01
 </t>
     </r>
     <r>
@@ -496,23 +562,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Each Secondary model was compared against the "Age + IHC" initial model. </t>
-    </r>
-  </si>
-  <si>
-    <t>Table 5</t>
-  </si>
-  <si>
-    <t>Has Successor knowledge</t>
-  </si>
-  <si>
-    <t>Has Endless knowledge</t>
-  </si>
-  <si>
-    <t>No Infinity knowledge</t>
-  </si>
-  <si>
-    <t>Table 2</t>
+      <t xml:space="preserve">Each Secondary model was compared against the "Age + IHC" initial model, and none explained significant additional variance. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -669,7 +720,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -847,6 +898,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1141,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A45" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A33" zoomScale="186" zoomScalePageLayoutView="186" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1406,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8">
         <v>29</v>
@@ -1380,7 +1434,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="10">
         <v>20</v>
@@ -1408,7 +1462,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="8">
         <v>10</v>
@@ -1436,7 +1490,7 @@
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7">
         <v>20</v>
@@ -1646,7 +1700,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="54"/>
@@ -1720,7 +1774,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -1748,14 +1802,14 @@
         <v>5</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,7 +1874,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1836,7 +1890,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B45" s="8">
         <v>59</v>
@@ -1848,7 +1902,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B46" s="10">
         <v>29</v>
@@ -1860,7 +1914,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B47" s="8">
         <v>11</v>
@@ -1872,7 +1926,7 @@
     </row>
     <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" s="7">
         <v>23</v>
@@ -1946,22 +2000,22 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B55" s="8">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C55" s="54">
         <f>B55/79</f>
-        <v>0.36708860759493672</v>
+        <v>0.34177215189873417</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F55" s="54">
         <f>E55/43</f>
-        <v>0.69767441860465118</v>
+        <v>0.7441860465116279</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8">
@@ -1973,17 +2027,17 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B56" s="10">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C56" s="56">
         <v>0.50600000000000001</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="10">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F56" s="56">
         <v>0.27900000000000003</v>
@@ -1998,7 +2052,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B57" s="10">
         <v>30</v>
@@ -2023,7 +2077,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="58" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B58" s="7">
         <v>20</v>
@@ -2051,6 +2105,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
@@ -2063,13 +2124,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2086,14 +2140,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A11" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
     <col min="8" max="8" width="12" style="9" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
@@ -2102,7 +2159,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2123,7 +2180,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -2131,37 +2188,37 @@
       <c r="F3" s="62"/>
       <c r="G3" s="11"/>
       <c r="H3" s="61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="61"/>
       <c r="J3" s="61"/>
     </row>
-    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2231,55 +2288,55 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B9" s="24">
-        <v>0.245</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24">
-        <v>0.27100000000000002</v>
+        <v>0.126</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="31">
-        <v>-80.61</v>
+        <v>-81.36</v>
       </c>
       <c r="I9" s="31">
-        <v>167.221</v>
+        <v>168.72</v>
       </c>
       <c r="J9" s="46">
-        <v>5.6000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="29">
-        <v>0.14899999999999999</v>
+        <v>0.193</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29">
-        <v>0.81599999999999995</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="33">
-        <v>-79.977000000000004</v>
+        <v>-80.73</v>
       </c>
       <c r="I10" s="33">
-        <v>165.95400000000001</v>
+        <v>167.45</v>
       </c>
       <c r="J10" s="46">
-        <v>7.0000000000000007E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="30">
         <v>0.217</v>
@@ -2288,22 +2345,22 @@
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="30">
-        <v>0.49359999999999998</v>
+        <v>0.221</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="34">
-        <v>-81.072000000000003</v>
+        <v>-81.069999999999993</v>
       </c>
       <c r="I11" s="34">
         <v>168.143</v>
       </c>
       <c r="J11" s="46">
-        <v>4.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="63"/>
       <c r="C12" s="63"/>
@@ -2348,14 +2405,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="10" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
     <col min="8" max="8" width="12" style="9" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
@@ -2364,12 +2424,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2385,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -2393,7 +2453,7 @@
       <c r="F3" s="62"/>
       <c r="G3" s="11"/>
       <c r="H3" s="61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="61"/>
       <c r="J3" s="61"/>
@@ -2404,26 +2464,26 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2436,7 +2496,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2475,14 +2535,14 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I8" s="32">
         <v>131.619</v>
@@ -2493,23 +2553,23 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.44800000000000001</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="42" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I9" s="31">
-        <v>133.767</v>
+        <v>131.786</v>
       </c>
       <c r="J9" s="39">
         <v>0.183</v>
@@ -2517,23 +2577,23 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="29">
-        <v>0.44600000000000001</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="64">
+        <v>0.36</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="43" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I10" s="33">
-        <v>134.19</v>
+        <v>131.37700000000001</v>
       </c>
       <c r="J10" s="39">
         <v>0.17899999999999999</v>
@@ -2541,23 +2601,23 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="29">
-        <v>0.30499999999999999</v>
+        <v>0.313</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="43" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="I11" s="33">
-        <v>130.624</v>
+        <v>130.971</v>
       </c>
       <c r="J11" s="39">
         <v>0.215</v>
@@ -2565,7 +2625,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2579,85 +2639,85 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B13" s="29">
-        <v>0.41099999999999998</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="C13" s="29">
-        <v>0.52900000000000003</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="D13" s="29">
-        <v>0.17299999999999999</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="33">
-        <v>-62.642000000000003</v>
+        <v>-62.204000000000001</v>
       </c>
       <c r="I13" s="33">
-        <v>133.28399999999999</v>
+        <v>132.40700000000001</v>
       </c>
       <c r="J13" s="39">
-        <v>0.20899999999999999</v>
+        <v>0.21809999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="29">
-        <v>0.315</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>43</v>
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0.43099999999999999</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29">
-        <v>0.82299999999999995</v>
+        <v>1.141</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="33">
-        <v>-62.058999999999997</v>
+      <c r="H14" s="43">
+        <v>-61.44</v>
       </c>
       <c r="I14" s="33">
-        <v>132.11799999999999</v>
+        <v>130.88300000000001</v>
       </c>
       <c r="J14" s="39">
-        <v>0.221</v>
+        <v>0.23300000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="39">
-        <v>0.249</v>
+        <v>0.25</v>
       </c>
       <c r="C15" s="39">
-        <v>0.40500000000000003</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="39">
-        <v>1.3877999999999999</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="G15" s="29"/>
       <c r="H15" s="33">
-        <v>-61.134999999999998</v>
+        <v>-61.295999999999999</v>
       </c>
       <c r="I15" s="33">
-        <v>130.47</v>
+        <v>130.59200000000001</v>
       </c>
       <c r="J15" s="39">
-        <v>0.23699999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="44" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.23599999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="44" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B16" s="63"/>
       <c r="C16" s="63"/>
@@ -2692,13 +2752,15 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.83203125" style="9" customWidth="1"/>
     <col min="8" max="8" width="12" style="9" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="9" customWidth="1"/>
@@ -2712,7 +2774,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -2728,7 +2790,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -2736,7 +2798,7 @@
       <c r="F3" s="62"/>
       <c r="G3" s="11"/>
       <c r="H3" s="61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="61"/>
       <c r="J3" s="61"/>
@@ -2747,26 +2809,26 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2779,7 +2841,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2815,7 +2877,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8" s="26">
         <v>0.38500000000000001</v>
@@ -2836,39 +2898,39 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.53200000000000003</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24">
-        <v>0.38300000000000001</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="31">
-        <v>-53.04</v>
+      <c r="H9" s="42" t="s">
+        <v>62</v>
       </c>
       <c r="I9" s="31">
-        <v>112.08</v>
+        <v>110.857</v>
       </c>
       <c r="J9" s="46">
-        <v>0.151</v>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="29">
+        <v>0.499</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29">
-        <v>0.90400000000000003</v>
+        <v>1.1779999999999999</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -2876,37 +2938,37 @@
         <v>-53.497</v>
       </c>
       <c r="I10" s="33">
-        <v>112.995</v>
+        <v>111.732</v>
       </c>
       <c r="J10" s="46">
-        <v>0.14000000000000001</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>49</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0.497</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="30">
-        <v>1.2729999999999999</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="34">
         <v>-52.970999999999997</v>
       </c>
       <c r="I11" s="34">
-        <v>111.94199999999999</v>
+        <v>112.129</v>
       </c>
       <c r="J11" s="46">
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="63" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
double-checked productivity coding and added justifications match methods section
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyichu/Sites/recursion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FD1C20-FF0A-1441-B3DF-B3869E1A668F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4908FEDE-2C89-9645-AE00-96E7B854FCFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33140" yWindow="-2260" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -884,6 +884,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -898,9 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1227,26 +1227,26 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="62"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="63"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62"/>
+      <c r="I3" s="63"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1363,26 +1363,26 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="62"/>
+      <c r="F11" s="63"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="62"/>
+      <c r="I11" s="63"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="60"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1533,26 +1533,26 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="62"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="62"/>
+      <c r="F20" s="63"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="62"/>
+      <c r="I20" s="63"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
@@ -1783,21 +1783,21 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="62"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="61" t="s">
+      <c r="E36" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="62"/>
+      <c r="F36" s="63"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="7" t="s">
         <v>5</v>
       </c>
@@ -1957,26 +1957,26 @@
       <c r="G52" s="20"/>
     </row>
     <row r="53" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="59" t="s">
+      <c r="A53" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="61" t="s">
+      <c r="B53" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="62"/>
+      <c r="C53" s="63"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="61" t="s">
+      <c r="E53" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="62"/>
+      <c r="F53" s="63"/>
       <c r="G53" s="11"/>
-      <c r="H53" s="61" t="s">
+      <c r="H53" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="62"/>
+      <c r="I53" s="63"/>
     </row>
     <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="7" t="s">
         <v>5</v>
       </c>
@@ -2105,13 +2105,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
@@ -2124,6 +2117,13 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2140,9 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2176,25 +2174,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
@@ -2359,18 +2357,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
@@ -2405,7 +2403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="168" zoomScalePageLayoutView="168" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:J16"/>
     </sheetView>
   </sheetViews>
@@ -2441,25 +2439,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
@@ -2579,7 +2577,7 @@
       <c r="A10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="64">
+      <c r="B10" s="59">
         <v>0.36</v>
       </c>
       <c r="C10" s="29"/>
@@ -2716,18 +2714,18 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="44" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2786,25 +2784,25 @@
       <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
@@ -2969,18 +2967,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>

</xml_diff>